<commit_message>
BOM done and minor changes
</commit_message>
<xml_diff>
--- a/Circuit/BOM/BOM.xlsx
+++ b/Circuit/BOM/BOM.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="41">
   <si>
     <t xml:space="preserve">No.</t>
   </si>
@@ -112,7 +112,7 @@
     <t xml:space="preserve">for AD7705 IC</t>
   </si>
   <si>
-    <t xml:space="preserve">JST 8-pin</t>
+    <t xml:space="preserve">GX16 – 8Pole connector</t>
   </si>
   <si>
     <t xml:space="preserve">for servo output</t>
@@ -134,6 +134,12 @@
   </si>
   <si>
     <t xml:space="preserve">PCB </t>
+  </si>
+  <si>
+    <t xml:space="preserve">&lt;&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Design, Manufacture and Testing</t>
   </si>
   <si>
     <t xml:space="preserve">TOTAL</t>
@@ -193,12 +199,18 @@
       <charset val="1"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor rgb="FFFFFF00"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="10">
@@ -298,7 +310,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="17">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -344,6 +356,18 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="2" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="2" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -372,16 +396,16 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:H25"/>
+  <dimension ref="A1:H27"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="180" zoomScaleNormal="180" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D3" activeCellId="0" sqref="D3"/>
+      <selection pane="topLeft" activeCell="D30" activeCellId="0" sqref="D30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.50390625" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.51171875" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="4"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="24.66"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="28.46"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="11"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="8.17"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="9.5"/>
@@ -420,13 +444,15 @@
       <c r="B2" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="C2" s="8"/>
+      <c r="C2" s="8" t="n">
+        <v>70</v>
+      </c>
       <c r="D2" s="8" t="n">
         <v>4</v>
       </c>
       <c r="E2" s="9" t="n">
         <f aca="false">C2*D2</f>
-        <v>0</v>
+        <v>280</v>
       </c>
       <c r="F2" s="8" t="s">
         <v>8</v>
@@ -441,13 +467,15 @@
       <c r="B3" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="C3" s="8"/>
+      <c r="C3" s="8" t="n">
+        <v>100</v>
+      </c>
       <c r="D3" s="8" t="n">
         <v>1</v>
       </c>
       <c r="E3" s="9" t="n">
         <f aca="false">C3*D3</f>
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="F3" s="8"/>
       <c r="G3" s="9"/>
@@ -460,13 +488,15 @@
       <c r="B4" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="C4" s="8"/>
+      <c r="C4" s="8" t="n">
+        <v>55</v>
+      </c>
       <c r="D4" s="8" t="n">
         <v>1</v>
       </c>
       <c r="E4" s="9" t="n">
         <f aca="false">C4*D4</f>
-        <v>0</v>
+        <v>55</v>
       </c>
       <c r="F4" s="8"/>
       <c r="G4" s="9"/>
@@ -479,7 +509,9 @@
       <c r="B5" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="C5" s="8"/>
+      <c r="C5" s="8" t="n">
+        <v>45</v>
+      </c>
       <c r="D5" s="8" t="n">
         <v>1</v>
       </c>
@@ -495,13 +527,15 @@
       <c r="B6" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="C6" s="8"/>
+      <c r="C6" s="8" t="n">
+        <v>10</v>
+      </c>
       <c r="D6" s="8" t="n">
-        <v>1</v>
+        <v>0.3</v>
       </c>
       <c r="E6" s="9" t="n">
         <f aca="false">C6*D6</f>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="F6" s="8"/>
       <c r="G6" s="9"/>
@@ -513,13 +547,15 @@
       <c r="B7" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="C7" s="8"/>
+      <c r="C7" s="8" t="n">
+        <v>0.75</v>
+      </c>
       <c r="D7" s="8" t="n">
         <v>3</v>
       </c>
       <c r="E7" s="9" t="n">
         <f aca="false">C7*D7</f>
-        <v>0</v>
+        <v>2.25</v>
       </c>
       <c r="F7" s="8" t="s">
         <v>14</v>
@@ -533,13 +569,15 @@
       <c r="B8" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="C8" s="8"/>
+      <c r="C8" s="8" t="n">
+        <v>10</v>
+      </c>
       <c r="D8" s="8" t="n">
         <v>1</v>
       </c>
       <c r="E8" s="9" t="n">
         <f aca="false">C8*D8</f>
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="F8" s="8"/>
       <c r="G8" s="9"/>
@@ -552,13 +590,15 @@
       <c r="B9" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="C9" s="8"/>
+      <c r="C9" s="8" t="n">
+        <v>1</v>
+      </c>
       <c r="D9" s="8" t="n">
         <v>1</v>
       </c>
       <c r="E9" s="9" t="n">
         <f aca="false">C9*D9</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F9" s="8" t="s">
         <v>17</v>
@@ -573,13 +613,15 @@
       <c r="B10" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="C10" s="8"/>
+      <c r="C10" s="8" t="n">
+        <v>5</v>
+      </c>
       <c r="D10" s="8" t="n">
         <v>1</v>
       </c>
       <c r="E10" s="9" t="n">
         <f aca="false">C10*D10</f>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="F10" s="8"/>
       <c r="G10" s="9"/>
@@ -592,13 +634,15 @@
       <c r="B11" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="C11" s="8"/>
+      <c r="C11" s="8" t="n">
+        <v>1</v>
+      </c>
       <c r="D11" s="8" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E11" s="9" t="n">
         <f aca="false">C11*D11</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F11" s="8" t="s">
         <v>20</v>
@@ -613,13 +657,15 @@
       <c r="B12" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="C12" s="8"/>
+      <c r="C12" s="8" t="n">
+        <v>1</v>
+      </c>
       <c r="D12" s="8" t="n">
         <v>1</v>
       </c>
       <c r="E12" s="9" t="n">
         <f aca="false">C12*D12</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F12" s="8" t="s">
         <v>22</v>
@@ -634,13 +680,15 @@
       <c r="B13" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="C13" s="8"/>
+      <c r="C13" s="8" t="n">
+        <v>5</v>
+      </c>
       <c r="D13" s="8" t="n">
         <v>2</v>
       </c>
       <c r="E13" s="9" t="n">
         <f aca="false">C13*D13</f>
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="F13" s="8" t="s">
         <v>24</v>
@@ -701,13 +749,15 @@
       <c r="B16" s="10" t="s">
         <v>28</v>
       </c>
-      <c r="C16" s="8"/>
+      <c r="C16" s="8" t="n">
+        <v>2</v>
+      </c>
       <c r="D16" s="8" t="n">
         <v>1</v>
       </c>
       <c r="E16" s="9" t="n">
         <f aca="false">C16*D16</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F16" s="8" t="s">
         <v>29</v>
@@ -722,13 +772,15 @@
       <c r="B17" s="10" t="s">
         <v>30</v>
       </c>
-      <c r="C17" s="8"/>
+      <c r="C17" s="8" t="n">
+        <v>60</v>
+      </c>
       <c r="D17" s="8" t="n">
         <v>1</v>
       </c>
       <c r="E17" s="9" t="n">
         <f aca="false">C17*D17</f>
-        <v>0</v>
+        <v>60</v>
       </c>
       <c r="F17" s="8" t="s">
         <v>31</v>
@@ -743,13 +795,15 @@
       <c r="B18" s="8" t="s">
         <v>32</v>
       </c>
-      <c r="C18" s="8"/>
+      <c r="C18" s="8" t="n">
+        <v>0.75</v>
+      </c>
       <c r="D18" s="8" t="n">
         <v>1</v>
       </c>
       <c r="E18" s="9" t="n">
         <f aca="false">C18*D18</f>
-        <v>0</v>
+        <v>0.75</v>
       </c>
       <c r="F18" s="8" t="s">
         <v>33</v>
@@ -764,13 +818,15 @@
       <c r="B19" s="8" t="s">
         <v>34</v>
       </c>
-      <c r="C19" s="8"/>
+      <c r="C19" s="8" t="n">
+        <v>0.5</v>
+      </c>
       <c r="D19" s="8" t="n">
         <v>1</v>
       </c>
       <c r="E19" s="9" t="n">
         <f aca="false">C19*D19</f>
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="F19" s="8"/>
       <c r="G19" s="9"/>
@@ -783,13 +839,15 @@
       <c r="B20" s="8" t="s">
         <v>35</v>
       </c>
-      <c r="C20" s="8"/>
+      <c r="C20" s="8" t="n">
+        <v>2.5</v>
+      </c>
       <c r="D20" s="8" t="n">
         <v>1</v>
       </c>
       <c r="E20" s="9" t="n">
         <f aca="false">C20*D20</f>
-        <v>0</v>
+        <v>2.5</v>
       </c>
       <c r="F20" s="8"/>
       <c r="G20" s="9"/>
@@ -802,13 +860,15 @@
       <c r="B21" s="8" t="s">
         <v>36</v>
       </c>
-      <c r="C21" s="8"/>
+      <c r="C21" s="8" t="n">
+        <v>25</v>
+      </c>
       <c r="D21" s="8" t="n">
         <v>1</v>
       </c>
       <c r="E21" s="9" t="n">
         <f aca="false">C21*D21</f>
-        <v>0</v>
+        <v>25</v>
       </c>
       <c r="F21" s="8"/>
       <c r="G21" s="9"/>
@@ -846,29 +906,55 @@
       <c r="H23" s="5"/>
     </row>
     <row r="24" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="1"/>
-      <c r="B24" s="2" t="s">
+      <c r="A24" s="12" t="s">
         <v>38</v>
       </c>
-      <c r="C24" s="2"/>
-      <c r="D24" s="2"/>
-      <c r="E24" s="1" t="n">
-        <f aca="false">SUM(E2:E23)</f>
-        <v>140</v>
-      </c>
-      <c r="F24" s="12"/>
-      <c r="G24" s="13"/>
+      <c r="B24" s="13" t="s">
+        <v>39</v>
+      </c>
+      <c r="C24" s="13"/>
+      <c r="D24" s="13"/>
+      <c r="E24" s="14" t="n">
+        <v>4000</v>
+      </c>
+      <c r="F24" s="8"/>
+      <c r="G24" s="9"/>
       <c r="H24" s="5"/>
     </row>
-    <row r="25" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="5"/>
-      <c r="B25" s="5"/>
-      <c r="C25" s="5"/>
-      <c r="D25" s="5"/>
-      <c r="E25" s="5"/>
-      <c r="F25" s="5"/>
-      <c r="G25" s="5"/>
+    <row r="25" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="11"/>
+      <c r="B25" s="8"/>
+      <c r="C25" s="8"/>
+      <c r="D25" s="8"/>
+      <c r="E25" s="9"/>
+      <c r="F25" s="8"/>
+      <c r="G25" s="9"/>
       <c r="H25" s="5"/>
+    </row>
+    <row r="26" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="1"/>
+      <c r="B26" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="C26" s="2"/>
+      <c r="D26" s="2"/>
+      <c r="E26" s="1" t="n">
+        <f aca="false">SUM(E2:E25)</f>
+        <v>4700</v>
+      </c>
+      <c r="F26" s="15"/>
+      <c r="G26" s="16"/>
+      <c r="H26" s="5"/>
+    </row>
+    <row r="27" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="5"/>
+      <c r="B27" s="5"/>
+      <c r="C27" s="5"/>
+      <c r="D27" s="5"/>
+      <c r="E27" s="5"/>
+      <c r="F27" s="5"/>
+      <c r="G27" s="5"/>
+      <c r="H27" s="5"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>